<commit_message>
Solicitud de Cambios a Requerimientos
</commit_message>
<xml_diff>
--- a/Area_de_Proceso-_REQM/SOLCREQM/SOLCREQM_V1.1_2015.xlsx
+++ b/Area_de_Proceso-_REQM/SOLCREQM/SOLCREQM_V1.1_2015.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thefa\Documents\GitHub\UTP-GPS-ALARM\Area_de_Proceso-_REQM\SOLCREQM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UTP-GPS-ALARM\UTP-GPS-ALARM\Area_de_Proceso-_REQM\SOLCREQM\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="600" windowWidth="20490" windowHeight="7650"/>
   </bookViews>
   <sheets>
     <sheet name="Historial de Revisiones" sheetId="1" r:id="rId1"/>
@@ -65,9 +65,6 @@
   </si>
   <si>
     <t>SOLCREQ Solicitud de Cambios de Requerimientos</t>
-  </si>
-  <si>
-    <t>Versión: 1.0</t>
   </si>
   <si>
     <t>Fecha Efectiva: 13/10/2015</t>
@@ -325,11 +322,14 @@
   <si>
     <t>Tener muchos modulos dificultaba y aumentaba las horas hombres y los procesos de Ingeneria de manera innecesaria afectando la eficiencia de tiempo involucrado en el desarrollo del Proyecto</t>
   </si>
+  <si>
+    <t>Versión: 1.1</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -978,6 +978,51 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -990,50 +1035,38 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="4" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1086,37 +1119,85 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="30" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="2" borderId="32" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="4" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="33" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1136,14 +1217,6 @@
     <xf numFmtId="0" fontId="12" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -1160,79 +1233,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="30" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="13" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="13" fillId="2" borderId="32" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="33" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1739,7 +1739,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:I12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D11" sqref="D11:D12"/>
     </sheetView>
   </sheetViews>
@@ -1751,57 +1751,57 @@
   <sheetData>
     <row r="1" spans="2:9" ht="15.75" thickBot="1"/>
     <row r="2" spans="2:9" ht="15" customHeight="1">
-      <c r="B2" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="22"/>
+      <c r="B2" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="19"/>
       <c r="I2" s="10"/>
     </row>
     <row r="3" spans="2:9" ht="15" customHeight="1">
-      <c r="B3" s="23"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="25"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="22"/>
       <c r="I3" s="10"/>
     </row>
     <row r="4" spans="2:9" ht="15" customHeight="1" thickBot="1">
-      <c r="B4" s="26"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="28"/>
+      <c r="B4" s="23"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="25"/>
       <c r="I4" s="10"/>
     </row>
     <row r="5" spans="2:9" ht="15.75" thickBot="1"/>
     <row r="6" spans="2:9" ht="16.5" customHeight="1">
-      <c r="B6" s="29" t="s">
+      <c r="B6" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="30"/>
-      <c r="D6" s="30"/>
-      <c r="E6" s="30"/>
-      <c r="F6" s="30"/>
-      <c r="G6" s="30"/>
-      <c r="H6" s="31"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="27"/>
+      <c r="F6" s="27"/>
+      <c r="G6" s="27"/>
+      <c r="H6" s="28"/>
     </row>
     <row r="7" spans="2:9" ht="15.75" thickBot="1">
-      <c r="B7" s="32"/>
-      <c r="C7" s="33"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="33"/>
-      <c r="F7" s="33"/>
-      <c r="G7" s="33"/>
-      <c r="H7" s="34"/>
+      <c r="B7" s="29"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="30"/>
+      <c r="H7" s="31"/>
     </row>
     <row r="8" spans="2:9" ht="24">
       <c r="B8" s="11" t="s">
@@ -1827,71 +1827,78 @@
       </c>
     </row>
     <row r="9" spans="2:9">
-      <c r="B9" s="17">
+      <c r="B9" s="32">
         <v>1</v>
       </c>
-      <c r="C9" s="18" t="s">
+      <c r="C9" s="33" t="s">
+        <v>79</v>
+      </c>
+      <c r="D9" s="34">
+        <v>42290</v>
+      </c>
+      <c r="E9" s="32" t="s">
+        <v>78</v>
+      </c>
+      <c r="F9" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="G9" s="32" t="s">
+        <v>81</v>
+      </c>
+      <c r="H9" s="32" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9">
+      <c r="B10" s="32"/>
+      <c r="C10" s="33"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="32"/>
+      <c r="H10" s="32"/>
+    </row>
+    <row r="11" spans="2:9">
+      <c r="B11" s="32">
+        <v>2</v>
+      </c>
+      <c r="C11" s="33" t="s">
         <v>80</v>
       </c>
-      <c r="D9" s="19">
-        <v>42290</v>
-      </c>
-      <c r="E9" s="17" t="s">
-        <v>79</v>
-      </c>
-      <c r="F9" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="G9" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="H9" s="17" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="10" spans="2:9">
-      <c r="B10" s="17"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="17"/>
-    </row>
-    <row r="11" spans="2:9">
-      <c r="B11" s="17">
-        <v>2</v>
-      </c>
-      <c r="C11" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="D11" s="19">
+      <c r="D11" s="34">
         <v>42320</v>
       </c>
-      <c r="E11" s="17" t="s">
-        <v>79</v>
-      </c>
-      <c r="F11" s="17" t="s">
+      <c r="E11" s="32" t="s">
+        <v>78</v>
+      </c>
+      <c r="F11" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="G11" s="17" t="s">
+      <c r="G11" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="H11" s="17" t="s">
-        <v>64</v>
+      <c r="H11" s="32" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="2:9">
-      <c r="B12" s="17"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="17"/>
+      <c r="B12" s="32"/>
+      <c r="C12" s="33"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="32"/>
+      <c r="G12" s="32"/>
+      <c r="H12" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="F11:F12"/>
     <mergeCell ref="B2:H4"/>
     <mergeCell ref="B6:H7"/>
     <mergeCell ref="B9:B10"/>
@@ -1901,13 +1908,6 @@
     <mergeCell ref="F9:F10"/>
     <mergeCell ref="G9:G10"/>
     <mergeCell ref="H9:H10"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="F11:F12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1918,8 +1918,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I29"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18:D18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E25" sqref="E25:G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1929,327 +1929,356 @@
   <sheetData>
     <row r="2" spans="2:9" ht="15.75" thickBot="1"/>
     <row r="3" spans="2:9" ht="15" customHeight="1">
-      <c r="C3" s="35" t="s">
-        <v>54</v>
-      </c>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
-      <c r="G3" s="37"/>
+      <c r="C3" s="46" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" s="47"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="48"/>
       <c r="H3" s="12"/>
       <c r="I3" s="12"/>
     </row>
     <row r="4" spans="2:9" ht="15" customHeight="1">
-      <c r="C4" s="38"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="39"/>
-      <c r="G4" s="40"/>
+      <c r="C4" s="49"/>
+      <c r="D4" s="50"/>
+      <c r="E4" s="50"/>
+      <c r="F4" s="50"/>
+      <c r="G4" s="51"/>
       <c r="H4" s="12"/>
       <c r="I4" s="12"/>
     </row>
     <row r="5" spans="2:9" ht="15.75" customHeight="1" thickBot="1">
       <c r="B5" s="1"/>
-      <c r="C5" s="41"/>
-      <c r="D5" s="42"/>
-      <c r="E5" s="42"/>
-      <c r="F5" s="42"/>
-      <c r="G5" s="43"/>
+      <c r="C5" s="52"/>
+      <c r="D5" s="53"/>
+      <c r="E5" s="53"/>
+      <c r="F5" s="53"/>
+      <c r="G5" s="54"/>
       <c r="H5" s="12"/>
       <c r="I5" s="12"/>
     </row>
     <row r="6" spans="2:9" ht="15" customHeight="1">
       <c r="B6" s="2"/>
-      <c r="C6" s="44" t="s">
+      <c r="C6" s="55" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="45"/>
-      <c r="E6" s="45"/>
-      <c r="F6" s="45"/>
-      <c r="G6" s="46"/>
+      <c r="D6" s="56"/>
+      <c r="E6" s="56"/>
+      <c r="F6" s="56"/>
+      <c r="G6" s="57"/>
     </row>
     <row r="7" spans="2:9" ht="25.5">
       <c r="B7" s="2"/>
       <c r="C7" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="D7" s="60" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="49" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" s="50"/>
-      <c r="F7" s="50"/>
-      <c r="G7" s="51"/>
+      <c r="E7" s="61"/>
+      <c r="F7" s="61"/>
+      <c r="G7" s="62"/>
     </row>
     <row r="8" spans="2:9">
       <c r="B8" s="3"/>
-      <c r="C8" s="47" t="s">
+      <c r="C8" s="58" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="59" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="48" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" s="48"/>
-      <c r="F8" s="48"/>
-      <c r="G8" s="48"/>
+      <c r="E8" s="59"/>
+      <c r="F8" s="59"/>
+      <c r="G8" s="59"/>
     </row>
     <row r="9" spans="2:9" ht="15" customHeight="1">
       <c r="B9" s="2"/>
-      <c r="C9" s="47"/>
-      <c r="D9" s="48"/>
-      <c r="E9" s="48"/>
-      <c r="F9" s="48"/>
-      <c r="G9" s="48"/>
+      <c r="C9" s="58"/>
+      <c r="D9" s="59"/>
+      <c r="E9" s="59"/>
+      <c r="F9" s="59"/>
+      <c r="G9" s="59"/>
     </row>
     <row r="10" spans="2:9" ht="7.5" customHeight="1">
       <c r="B10" s="2"/>
-      <c r="C10" s="47"/>
-      <c r="D10" s="48"/>
-      <c r="E10" s="48"/>
-      <c r="F10" s="48"/>
-      <c r="G10" s="48"/>
+      <c r="C10" s="58"/>
+      <c r="D10" s="59"/>
+      <c r="E10" s="59"/>
+      <c r="F10" s="59"/>
+      <c r="G10" s="59"/>
     </row>
     <row r="11" spans="2:9" hidden="1">
       <c r="B11" s="2"/>
-      <c r="C11" s="47"/>
-      <c r="D11" s="48"/>
-      <c r="E11" s="48"/>
-      <c r="F11" s="48"/>
-      <c r="G11" s="48"/>
+      <c r="C11" s="58"/>
+      <c r="D11" s="59"/>
+      <c r="E11" s="59"/>
+      <c r="F11" s="59"/>
+      <c r="G11" s="59"/>
     </row>
     <row r="12" spans="2:9" hidden="1">
       <c r="B12" s="4"/>
-      <c r="C12" s="47"/>
-      <c r="D12" s="48"/>
-      <c r="E12" s="48"/>
-      <c r="F12" s="48"/>
-      <c r="G12" s="48"/>
+      <c r="C12" s="58"/>
+      <c r="D12" s="59"/>
+      <c r="E12" s="59"/>
+      <c r="F12" s="59"/>
+      <c r="G12" s="59"/>
     </row>
     <row r="13" spans="2:9">
       <c r="B13" s="5"/>
-      <c r="C13" s="54" t="s">
-        <v>17</v>
-      </c>
-      <c r="D13" s="54"/>
-      <c r="E13" s="54"/>
-      <c r="F13" s="54"/>
-      <c r="G13" s="54"/>
+      <c r="C13" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="42"/>
+      <c r="E13" s="42"/>
+      <c r="F13" s="42"/>
+      <c r="G13" s="42"/>
     </row>
     <row r="14" spans="2:9">
       <c r="B14" s="5"/>
-      <c r="C14" s="55" t="s">
-        <v>16</v>
-      </c>
-      <c r="D14" s="56"/>
-      <c r="E14" s="57" t="s">
+      <c r="C14" s="43" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="44"/>
+      <c r="E14" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="F14" s="57"/>
-      <c r="G14" s="57"/>
+      <c r="F14" s="45"/>
+      <c r="G14" s="45"/>
     </row>
     <row r="15" spans="2:9">
       <c r="B15" s="4"/>
-      <c r="C15" s="52" t="s">
-        <v>18</v>
-      </c>
-      <c r="D15" s="52"/>
-      <c r="E15" s="53"/>
-      <c r="F15" s="53"/>
-      <c r="G15" s="53"/>
+      <c r="C15" s="40" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" s="40"/>
+      <c r="E15" s="41"/>
+      <c r="F15" s="41"/>
+      <c r="G15" s="41"/>
     </row>
     <row r="16" spans="2:9" ht="24.95" customHeight="1">
       <c r="B16" s="6"/>
-      <c r="C16" s="58" t="s">
+      <c r="C16" s="38" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" s="39"/>
+      <c r="E16" s="37" t="s">
+        <v>75</v>
+      </c>
+      <c r="F16" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="D16" s="59"/>
-      <c r="E16" s="60" t="s">
-        <v>76</v>
-      </c>
-      <c r="F16" s="60" t="s">
-        <v>20</v>
-      </c>
-      <c r="G16" s="60"/>
+      <c r="G16" s="37"/>
     </row>
     <row r="17" spans="2:7" ht="24.95" customHeight="1">
       <c r="B17" s="6"/>
-      <c r="C17" s="58" t="s">
+      <c r="C17" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" s="39"/>
+      <c r="E17" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="D17" s="59"/>
-      <c r="E17" s="60" t="s">
-        <v>22</v>
-      </c>
-      <c r="F17" s="60" t="s">
-        <v>21</v>
-      </c>
-      <c r="G17" s="60"/>
+      <c r="F17" s="37" t="s">
+        <v>20</v>
+      </c>
+      <c r="G17" s="37"/>
     </row>
     <row r="18" spans="2:7" ht="24.95" customHeight="1">
       <c r="B18" s="6"/>
-      <c r="C18" s="58" t="s">
+      <c r="C18" s="38" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" s="39"/>
+      <c r="E18" s="37" t="s">
+        <v>83</v>
+      </c>
+      <c r="F18" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="D18" s="59"/>
-      <c r="E18" s="60" t="s">
-        <v>84</v>
-      </c>
-      <c r="F18" s="60" t="s">
-        <v>24</v>
-      </c>
-      <c r="G18" s="60"/>
+      <c r="G18" s="37"/>
     </row>
     <row r="19" spans="2:7" ht="24.95" customHeight="1">
       <c r="B19" s="6"/>
-      <c r="C19" s="58" t="s">
+      <c r="C19" s="38" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19" s="39"/>
+      <c r="E19" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="D19" s="59"/>
-      <c r="E19" s="60" t="s">
+      <c r="F19" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="F19" s="60" t="s">
-        <v>27</v>
-      </c>
-      <c r="G19" s="60"/>
+      <c r="G19" s="37"/>
     </row>
     <row r="20" spans="2:7" ht="24.95" customHeight="1">
       <c r="B20" s="6"/>
-      <c r="C20" s="58" t="s">
+      <c r="C20" s="38" t="s">
+        <v>27</v>
+      </c>
+      <c r="D20" s="39"/>
+      <c r="E20" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="D20" s="59"/>
-      <c r="E20" s="60" t="s">
-        <v>29</v>
-      </c>
-      <c r="F20" s="60" t="s">
-        <v>29</v>
-      </c>
-      <c r="G20" s="60"/>
+      <c r="F20" s="37" t="s">
+        <v>28</v>
+      </c>
+      <c r="G20" s="37"/>
     </row>
     <row r="21" spans="2:7" ht="24.95" customHeight="1">
       <c r="B21" s="6"/>
-      <c r="C21" s="58" t="s">
+      <c r="C21" s="38" t="s">
+        <v>29</v>
+      </c>
+      <c r="D21" s="39"/>
+      <c r="E21" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="D21" s="59"/>
-      <c r="E21" s="60" t="s">
+      <c r="F21" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="F21" s="60" t="s">
-        <v>32</v>
-      </c>
-      <c r="G21" s="60"/>
+      <c r="G21" s="37"/>
     </row>
     <row r="22" spans="2:7" ht="24.95" customHeight="1">
       <c r="B22" s="6"/>
-      <c r="C22" s="58" t="s">
+      <c r="C22" s="38" t="s">
+        <v>32</v>
+      </c>
+      <c r="D22" s="39"/>
+      <c r="E22" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="D22" s="59"/>
-      <c r="E22" s="60" t="s">
-        <v>34</v>
-      </c>
-      <c r="F22" s="60"/>
-      <c r="G22" s="60"/>
+      <c r="F22" s="37"/>
+      <c r="G22" s="37"/>
     </row>
     <row r="23" spans="2:7" ht="24.95" customHeight="1">
       <c r="B23" s="6"/>
-      <c r="C23" s="58" t="s">
+      <c r="C23" s="38" t="s">
+        <v>34</v>
+      </c>
+      <c r="D23" s="39"/>
+      <c r="E23" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="D23" s="59"/>
-      <c r="E23" s="60" t="s">
-        <v>36</v>
-      </c>
-      <c r="F23" s="60"/>
-      <c r="G23" s="60"/>
+      <c r="F23" s="37"/>
+      <c r="G23" s="37"/>
     </row>
     <row r="24" spans="2:7" ht="24.95" customHeight="1">
       <c r="B24" s="7"/>
-      <c r="C24" s="58" t="s">
+      <c r="C24" s="38" t="s">
+        <v>36</v>
+      </c>
+      <c r="D24" s="39"/>
+      <c r="E24" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="D24" s="59"/>
-      <c r="E24" s="60" t="s">
+      <c r="F24" s="37" t="s">
         <v>38</v>
       </c>
-      <c r="F24" s="60" t="s">
-        <v>39</v>
-      </c>
-      <c r="G24" s="60"/>
+      <c r="G24" s="37"/>
     </row>
     <row r="25" spans="2:7" ht="24.95" customHeight="1">
       <c r="B25" s="7"/>
-      <c r="C25" s="58" t="s">
-        <v>14</v>
-      </c>
-      <c r="D25" s="59"/>
-      <c r="E25" s="60" t="s">
+      <c r="C25" s="38" t="s">
+        <v>13</v>
+      </c>
+      <c r="D25" s="39"/>
+      <c r="E25" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="F25" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="F25" s="60" t="s">
-        <v>41</v>
-      </c>
-      <c r="G25" s="60"/>
+      <c r="G25" s="37"/>
     </row>
     <row r="26" spans="2:7" ht="24.95" customHeight="1">
       <c r="B26" s="6"/>
-      <c r="C26" s="58" t="s">
+      <c r="C26" s="38" t="s">
+        <v>41</v>
+      </c>
+      <c r="D26" s="39"/>
+      <c r="E26" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="D26" s="59"/>
-      <c r="E26" s="60" t="s">
+      <c r="F26" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="F26" s="60" t="s">
-        <v>44</v>
-      </c>
-      <c r="G26" s="60"/>
+      <c r="G26" s="37"/>
     </row>
     <row r="27" spans="2:7" ht="24.95" customHeight="1">
       <c r="B27" s="7"/>
-      <c r="C27" s="58" t="s">
+      <c r="C27" s="38" t="s">
+        <v>44</v>
+      </c>
+      <c r="D27" s="39"/>
+      <c r="E27" s="37" t="s">
         <v>45</v>
       </c>
-      <c r="D27" s="59"/>
-      <c r="E27" s="60" t="s">
+      <c r="F27" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="F27" s="60" t="s">
-        <v>47</v>
-      </c>
-      <c r="G27" s="60"/>
+      <c r="G27" s="37"/>
     </row>
     <row r="28" spans="2:7" ht="24.95" customHeight="1">
       <c r="B28" s="6"/>
-      <c r="C28" s="58" t="s">
+      <c r="C28" s="38" t="s">
+        <v>47</v>
+      </c>
+      <c r="D28" s="39"/>
+      <c r="E28" s="37" t="s">
         <v>48</v>
       </c>
-      <c r="D28" s="59"/>
-      <c r="E28" s="60" t="s">
+      <c r="F28" s="37" t="s">
         <v>49</v>
       </c>
-      <c r="F28" s="60" t="s">
-        <v>50</v>
-      </c>
-      <c r="G28" s="60"/>
+      <c r="G28" s="37"/>
     </row>
     <row r="29" spans="2:7" ht="24.95" customHeight="1">
       <c r="B29" s="8"/>
-      <c r="C29" s="61" t="s">
+      <c r="C29" s="35" t="s">
+        <v>50</v>
+      </c>
+      <c r="D29" s="36"/>
+      <c r="E29" s="37" t="s">
         <v>51</v>
       </c>
-      <c r="D29" s="62"/>
-      <c r="E29" s="60" t="s">
+      <c r="F29" s="37" t="s">
         <v>52</v>
       </c>
-      <c r="F29" s="60" t="s">
-        <v>53</v>
-      </c>
-      <c r="G29" s="60"/>
+      <c r="G29" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="37">
+    <mergeCell ref="C3:G5"/>
+    <mergeCell ref="C6:G6"/>
+    <mergeCell ref="C8:C12"/>
+    <mergeCell ref="D8:G12"/>
+    <mergeCell ref="D7:G7"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="E17:G17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="E18:G18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="E19:G19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="E20:G20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="E21:G21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="E22:G22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="E28:G28"/>
     <mergeCell ref="C29:D29"/>
     <mergeCell ref="E29:G29"/>
     <mergeCell ref="C25:D25"/>
@@ -2258,35 +2287,6 @@
     <mergeCell ref="E26:G26"/>
     <mergeCell ref="C27:D27"/>
     <mergeCell ref="E27:G27"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="E24:G24"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="E28:G28"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="E20:G20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="E21:G21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="E22:G22"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="E17:G17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="E18:G18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="E19:G19"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="C13:G13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="C3:G5"/>
-    <mergeCell ref="C6:G6"/>
-    <mergeCell ref="C8:C12"/>
-    <mergeCell ref="D8:G12"/>
-    <mergeCell ref="D7:G7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -2298,7 +2298,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B24" sqref="B24:D24"/>
     </sheetView>
   </sheetViews>
@@ -2319,205 +2319,212 @@
     </row>
     <row r="2" spans="1:7" ht="15" customHeight="1">
       <c r="A2" s="9"/>
-      <c r="B2" s="75" t="s">
-        <v>54</v>
-      </c>
-      <c r="C2" s="76"/>
-      <c r="D2" s="77"/>
+      <c r="B2" s="63" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" s="64"/>
+      <c r="D2" s="65"/>
       <c r="E2" s="14"/>
       <c r="F2" s="14"/>
       <c r="G2" s="10"/>
     </row>
     <row r="3" spans="1:7" ht="15" customHeight="1">
       <c r="A3" s="9"/>
-      <c r="B3" s="78"/>
-      <c r="C3" s="79"/>
-      <c r="D3" s="80"/>
+      <c r="B3" s="66"/>
+      <c r="C3" s="67"/>
+      <c r="D3" s="68"/>
       <c r="E3" s="14"/>
       <c r="F3" s="14"/>
       <c r="G3" s="10"/>
     </row>
     <row r="4" spans="1:7" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B4" s="81"/>
-      <c r="C4" s="82"/>
-      <c r="D4" s="83"/>
+      <c r="B4" s="69"/>
+      <c r="C4" s="70"/>
+      <c r="D4" s="71"/>
       <c r="E4" s="14"/>
       <c r="F4" s="14"/>
     </row>
     <row r="5" spans="1:7" ht="18">
-      <c r="B5" s="65" t="s">
+      <c r="B5" s="89" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" s="90"/>
+      <c r="D5" s="91"/>
+    </row>
+    <row r="6" spans="1:7" ht="15.75">
+      <c r="B6" s="94" t="s">
         <v>55</v>
       </c>
-      <c r="C5" s="66"/>
-      <c r="D5" s="67"/>
-    </row>
-    <row r="6" spans="1:7" ht="15.75">
-      <c r="B6" s="72" t="s">
-        <v>56</v>
-      </c>
-      <c r="C6" s="73"/>
-      <c r="D6" s="74"/>
+      <c r="C6" s="95"/>
+      <c r="D6" s="96"/>
     </row>
     <row r="7" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="B7" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7" s="74" t="s">
         <v>57</v>
       </c>
-      <c r="C7" s="68" t="s">
-        <v>58</v>
-      </c>
-      <c r="D7" s="69"/>
+      <c r="D7" s="75"/>
     </row>
     <row r="8" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="B8" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="C8" s="68" t="s">
+        <v>58</v>
+      </c>
+      <c r="C8" s="74" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="69"/>
+      <c r="D8" s="75"/>
     </row>
     <row r="9" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="B9" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="C9" s="92" t="s">
         <v>60</v>
       </c>
-      <c r="C9" s="70" t="s">
-        <v>61</v>
-      </c>
-      <c r="D9" s="71"/>
+      <c r="D9" s="93"/>
     </row>
     <row r="10" spans="1:7" ht="32.25" customHeight="1">
       <c r="B10" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="C10" s="84">
+        <v>61</v>
+      </c>
+      <c r="C10" s="72">
         <v>42290</v>
       </c>
-      <c r="D10" s="85"/>
+      <c r="D10" s="73"/>
     </row>
     <row r="11" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="B11" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="C11" s="74" t="s">
         <v>63</v>
       </c>
-      <c r="C11" s="68" t="s">
-        <v>64</v>
-      </c>
-      <c r="D11" s="69"/>
+      <c r="D11" s="75"/>
     </row>
     <row r="12" spans="1:7" ht="33" customHeight="1">
       <c r="B12" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="C12" s="74" t="s">
         <v>65</v>
       </c>
-      <c r="C12" s="68" t="s">
-        <v>66</v>
-      </c>
-      <c r="D12" s="69"/>
+      <c r="D12" s="75"/>
     </row>
     <row r="13" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="B13" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="C13" s="92" t="s">
         <v>67</v>
       </c>
-      <c r="C13" s="70" t="s">
-        <v>68</v>
-      </c>
-      <c r="D13" s="71"/>
+      <c r="D13" s="93"/>
     </row>
     <row r="14" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="B14" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="C14" s="63" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="87" t="s">
+        <v>84</v>
+      </c>
+      <c r="D14" s="88"/>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="B15" s="78" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="79"/>
+      <c r="D15" s="80"/>
+    </row>
+    <row r="16" spans="1:7" ht="50.1" customHeight="1">
+      <c r="B16" s="81" t="s">
+        <v>68</v>
+      </c>
+      <c r="C16" s="82"/>
+      <c r="D16" s="83"/>
+    </row>
+    <row r="17" spans="2:4">
+      <c r="B17" s="78" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" s="79"/>
+      <c r="D17" s="80"/>
+    </row>
+    <row r="18" spans="2:4" ht="50.1" customHeight="1">
+      <c r="B18" s="81" t="s">
+        <v>69</v>
+      </c>
+      <c r="C18" s="82"/>
+      <c r="D18" s="83"/>
+    </row>
+    <row r="19" spans="2:4">
+      <c r="B19" s="78" t="s">
+        <v>70</v>
+      </c>
+      <c r="C19" s="79"/>
+      <c r="D19" s="80"/>
+    </row>
+    <row r="20" spans="2:4" ht="50.1" customHeight="1">
+      <c r="B20" s="81" t="s">
         <v>85</v>
       </c>
-      <c r="D14" s="64"/>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="B15" s="88" t="s">
-        <v>37</v>
-      </c>
-      <c r="C15" s="89"/>
-      <c r="D15" s="90"/>
-    </row>
-    <row r="16" spans="1:7" ht="50.1" customHeight="1">
-      <c r="B16" s="91" t="s">
-        <v>69</v>
-      </c>
-      <c r="C16" s="92"/>
-      <c r="D16" s="93"/>
-    </row>
-    <row r="17" spans="2:4">
-      <c r="B17" s="88" t="s">
-        <v>14</v>
-      </c>
-      <c r="C17" s="89"/>
-      <c r="D17" s="90"/>
-    </row>
-    <row r="18" spans="2:4" ht="50.1" customHeight="1">
-      <c r="B18" s="91" t="s">
-        <v>70</v>
-      </c>
-      <c r="C18" s="92"/>
-      <c r="D18" s="93"/>
-    </row>
-    <row r="19" spans="2:4">
-      <c r="B19" s="88" t="s">
+      <c r="C20" s="82"/>
+      <c r="D20" s="83"/>
+    </row>
+    <row r="21" spans="2:4">
+      <c r="B21" s="78" t="s">
         <v>71</v>
       </c>
-      <c r="C19" s="89"/>
-      <c r="D19" s="90"/>
-    </row>
-    <row r="20" spans="2:4" ht="50.1" customHeight="1">
-      <c r="B20" s="91" t="s">
-        <v>86</v>
-      </c>
-      <c r="C20" s="92"/>
-      <c r="D20" s="93"/>
-    </row>
-    <row r="21" spans="2:4">
-      <c r="B21" s="88" t="s">
+      <c r="C21" s="79"/>
+      <c r="D21" s="80"/>
+    </row>
+    <row r="22" spans="2:4" ht="50.1" customHeight="1">
+      <c r="B22" s="81" t="s">
+        <v>76</v>
+      </c>
+      <c r="C22" s="82"/>
+      <c r="D22" s="83"/>
+    </row>
+    <row r="23" spans="2:4">
+      <c r="B23" s="78" t="s">
+        <v>47</v>
+      </c>
+      <c r="C23" s="79"/>
+      <c r="D23" s="80"/>
+    </row>
+    <row r="24" spans="2:4" ht="50.1" customHeight="1">
+      <c r="B24" s="81" t="s">
         <v>72</v>
       </c>
-      <c r="C21" s="89"/>
-      <c r="D21" s="90"/>
-    </row>
-    <row r="22" spans="2:4" ht="50.1" customHeight="1">
-      <c r="B22" s="91" t="s">
-        <v>77</v>
-      </c>
-      <c r="C22" s="92"/>
-      <c r="D22" s="93"/>
-    </row>
-    <row r="23" spans="2:4">
-      <c r="B23" s="88" t="s">
-        <v>48</v>
-      </c>
-      <c r="C23" s="89"/>
-      <c r="D23" s="90"/>
-    </row>
-    <row r="24" spans="2:4" ht="50.1" customHeight="1">
-      <c r="B24" s="91" t="s">
+      <c r="C24" s="82"/>
+      <c r="D24" s="83"/>
+    </row>
+    <row r="25" spans="2:4" ht="15.75" thickBot="1">
+      <c r="B25" s="84" t="s">
         <v>73</v>
       </c>
-      <c r="C24" s="92"/>
-      <c r="D24" s="93"/>
-    </row>
-    <row r="25" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B25" s="94" t="s">
-        <v>74</v>
-      </c>
-      <c r="C25" s="95"/>
-      <c r="D25" s="96"/>
+      <c r="C25" s="85"/>
+      <c r="D25" s="86"/>
     </row>
     <row r="26" spans="2:4" ht="26.25" thickBot="1">
       <c r="B26" s="15" t="s">
-        <v>75</v>
-      </c>
-      <c r="C26" s="86" t="s">
-        <v>78</v>
-      </c>
-      <c r="D26" s="87"/>
+        <v>74</v>
+      </c>
+      <c r="C26" s="76" t="s">
+        <v>77</v>
+      </c>
+      <c r="D26" s="77"/>
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="C13:D13"/>
     <mergeCell ref="B2:D4"/>
     <mergeCell ref="C10:D10"/>
     <mergeCell ref="C11:D11"/>
@@ -2534,13 +2541,6 @@
     <mergeCell ref="B23:D23"/>
     <mergeCell ref="B24:D24"/>
     <mergeCell ref="B25:D25"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="C13:D13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Solicitud de Cambios de Requerimientos
Actualizado
</commit_message>
<xml_diff>
--- a/Area_de_Proceso-_REQM/SOLCREQM/SOLCREQM_V1.1_2015.xlsx
+++ b/Area_de_Proceso-_REQM/SOLCREQM/SOLCREQM_V1.1_2015.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UTP-GPS-ALARM\UTP-GPS-ALARM\Area_de_Proceso-_REQM\SOLCREQM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jleonardo\Documents\GitHub\UTP-GPS-ALARM\Area_de_Proceso-_REQM\SOLCREQM\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="600" windowWidth="20490" windowHeight="7650"/>
+    <workbookView xWindow="0" yWindow="600" windowWidth="20490" windowHeight="7650" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Historial de Revisiones" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="95">
   <si>
     <t>HISTORIAL DE LAS REVISIONES</t>
   </si>
@@ -226,9 +226,6 @@
     <t xml:space="preserve">Personal que autoriza la Solicitud: </t>
   </si>
   <si>
-    <t>Roger Apaestegui Ortega</t>
-  </si>
-  <si>
     <t xml:space="preserve">Nombre del Proceso: </t>
   </si>
   <si>
@@ -245,9 +242,6 @@
   </si>
   <si>
     <t>Áreas Involucradas (stakeholders)</t>
-  </si>
-  <si>
-    <t>Este cambio generará un gran impácto en el desarrollo de la aplicación, se debe hacer los cambios y correcciones necesarias en Cronograma de Proyecto y Plan de Proyecto lo más antes posible, después de su aprobación.</t>
   </si>
   <si>
     <t>Documentos adjuntos</t>
@@ -324,6 +318,36 @@
   </si>
   <si>
     <t>Versión: 1.1</t>
+  </si>
+  <si>
+    <t>Roger Apaéstegui Ortega</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Este cambio generará un gran impácto en el desarrollo de la aplicación, se debe hacer los cambios y correcciones necesarias en los siguientes documentos inmediatamente después de su aprobación :  </t>
+  </si>
+  <si>
+    <t>1. PPROY_Plan de Proyecto</t>
+  </si>
+  <si>
+    <t>2. CPROY_Cronograma del Proyecto</t>
+  </si>
+  <si>
+    <t>3. LMREQM_Lista Maestra de Requerimientos</t>
+  </si>
+  <si>
+    <t>4. MTREQM_Matriz de Trazabilidad de Requerimientos</t>
+  </si>
+  <si>
+    <t>5. Registro de Cambios en los Requerimientos</t>
+  </si>
+  <si>
+    <t>6. REGRI_Registro de Riesgos</t>
+  </si>
+  <si>
+    <t>7. TABME_Tablero de Métricas</t>
+  </si>
+  <si>
+    <t>8. FMVREQM_Ficha de Métrica de Volatilidad de Requerimientos</t>
   </si>
 </sst>
 </file>
@@ -482,7 +506,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="36">
+  <borders count="39">
     <border>
       <left/>
       <right/>
@@ -926,6 +950,39 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -937,7 +994,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3" applyFont="1"/>
@@ -978,51 +1035,6 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -1035,89 +1047,176 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="19" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="4" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="4" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="19" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1154,14 +1253,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -1200,39 +1291,50 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="36" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="38" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1739,7 +1841,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11:D12"/>
     </sheetView>
   </sheetViews>
@@ -1751,57 +1853,57 @@
   <sheetData>
     <row r="1" spans="2:9" ht="15.75" thickBot="1"/>
     <row r="2" spans="2:9" ht="15" customHeight="1">
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="19"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="22"/>
       <c r="I2" s="10"/>
     </row>
     <row r="3" spans="2:9" ht="15" customHeight="1">
-      <c r="B3" s="20"/>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="22"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="25"/>
       <c r="I3" s="10"/>
     </row>
     <row r="4" spans="2:9" ht="15" customHeight="1" thickBot="1">
-      <c r="B4" s="23"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="25"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="28"/>
       <c r="I4" s="10"/>
     </row>
     <row r="5" spans="2:9" ht="15.75" thickBot="1"/>
     <row r="6" spans="2:9" ht="16.5" customHeight="1">
-      <c r="B6" s="26" t="s">
+      <c r="B6" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="27"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="27"/>
-      <c r="G6" s="27"/>
-      <c r="H6" s="28"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="31"/>
     </row>
     <row r="7" spans="2:9" ht="15.75" thickBot="1">
-      <c r="B7" s="29"/>
-      <c r="C7" s="30"/>
-      <c r="D7" s="30"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="30"/>
-      <c r="G7" s="30"/>
-      <c r="H7" s="31"/>
+      <c r="B7" s="32"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="33"/>
+      <c r="F7" s="33"/>
+      <c r="G7" s="33"/>
+      <c r="H7" s="34"/>
     </row>
     <row r="8" spans="2:9" ht="24">
       <c r="B8" s="11" t="s">
@@ -1827,78 +1929,71 @@
       </c>
     </row>
     <row r="9" spans="2:9">
-      <c r="B9" s="32">
+      <c r="B9" s="17">
         <v>1</v>
       </c>
-      <c r="C9" s="33" t="s">
+      <c r="C9" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="D9" s="19">
+        <v>42290</v>
+      </c>
+      <c r="E9" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="F9" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="G9" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="D9" s="34">
-        <v>42290</v>
-      </c>
-      <c r="E9" s="32" t="s">
+      <c r="H9" s="17" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9">
+      <c r="B10" s="17"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="17"/>
+    </row>
+    <row r="11" spans="2:9">
+      <c r="B11" s="17">
+        <v>2</v>
+      </c>
+      <c r="C11" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="F9" s="32" t="s">
-        <v>82</v>
-      </c>
-      <c r="G9" s="32" t="s">
-        <v>81</v>
-      </c>
-      <c r="H9" s="32" t="s">
+      <c r="D11" s="19">
+        <v>42320</v>
+      </c>
+      <c r="E11" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="F11" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="G11" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="H11" s="17" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="10" spans="2:9">
-      <c r="B10" s="32"/>
-      <c r="C10" s="33"/>
-      <c r="D10" s="32"/>
-      <c r="E10" s="32"/>
-      <c r="F10" s="32"/>
-      <c r="G10" s="32"/>
-      <c r="H10" s="32"/>
-    </row>
-    <row r="11" spans="2:9">
-      <c r="B11" s="32">
-        <v>2</v>
-      </c>
-      <c r="C11" s="33" t="s">
-        <v>80</v>
-      </c>
-      <c r="D11" s="34">
-        <v>42320</v>
-      </c>
-      <c r="E11" s="32" t="s">
-        <v>78</v>
-      </c>
-      <c r="F11" s="32" t="s">
-        <v>8</v>
-      </c>
-      <c r="G11" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="H11" s="32" t="s">
-        <v>63</v>
-      </c>
-    </row>
     <row r="12" spans="2:9">
-      <c r="B12" s="32"/>
-      <c r="C12" s="33"/>
-      <c r="D12" s="32"/>
-      <c r="E12" s="32"/>
-      <c r="F12" s="32"/>
-      <c r="G12" s="32"/>
-      <c r="H12" s="32"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="F11:F12"/>
     <mergeCell ref="B2:H4"/>
     <mergeCell ref="B6:H7"/>
     <mergeCell ref="B9:B10"/>
@@ -1908,6 +2003,13 @@
     <mergeCell ref="F9:F10"/>
     <mergeCell ref="G9:G10"/>
     <mergeCell ref="H9:H10"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="F11:F12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1918,7 +2020,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="E25" sqref="E25:G26"/>
     </sheetView>
   </sheetViews>
@@ -1929,356 +2031,327 @@
   <sheetData>
     <row r="2" spans="2:9" ht="15.75" thickBot="1"/>
     <row r="3" spans="2:9" ht="15" customHeight="1">
-      <c r="C3" s="46" t="s">
+      <c r="C3" s="35" t="s">
         <v>53</v>
       </c>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="47"/>
-      <c r="G3" s="48"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="37"/>
       <c r="H3" s="12"/>
       <c r="I3" s="12"/>
     </row>
     <row r="4" spans="2:9" ht="15" customHeight="1">
-      <c r="C4" s="49"/>
-      <c r="D4" s="50"/>
-      <c r="E4" s="50"/>
-      <c r="F4" s="50"/>
-      <c r="G4" s="51"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="40"/>
       <c r="H4" s="12"/>
       <c r="I4" s="12"/>
     </row>
     <row r="5" spans="2:9" ht="15.75" customHeight="1" thickBot="1">
       <c r="B5" s="1"/>
-      <c r="C5" s="52"/>
-      <c r="D5" s="53"/>
-      <c r="E5" s="53"/>
-      <c r="F5" s="53"/>
-      <c r="G5" s="54"/>
+      <c r="C5" s="41"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="43"/>
       <c r="H5" s="12"/>
       <c r="I5" s="12"/>
     </row>
     <row r="6" spans="2:9" ht="15" customHeight="1">
       <c r="B6" s="2"/>
-      <c r="C6" s="55" t="s">
+      <c r="C6" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="56"/>
-      <c r="E6" s="56"/>
-      <c r="F6" s="56"/>
-      <c r="G6" s="57"/>
+      <c r="D6" s="45"/>
+      <c r="E6" s="45"/>
+      <c r="F6" s="45"/>
+      <c r="G6" s="46"/>
     </row>
     <row r="7" spans="2:9" ht="25.5">
       <c r="B7" s="2"/>
       <c r="C7" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="D7" s="60" t="s">
+        <v>84</v>
+      </c>
+      <c r="D7" s="49" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="61"/>
-      <c r="F7" s="61"/>
-      <c r="G7" s="62"/>
+      <c r="E7" s="50"/>
+      <c r="F7" s="50"/>
+      <c r="G7" s="51"/>
     </row>
     <row r="8" spans="2:9">
       <c r="B8" s="3"/>
-      <c r="C8" s="58" t="s">
+      <c r="C8" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="59" t="s">
+      <c r="D8" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="59"/>
-      <c r="F8" s="59"/>
-      <c r="G8" s="59"/>
+      <c r="E8" s="48"/>
+      <c r="F8" s="48"/>
+      <c r="G8" s="48"/>
     </row>
     <row r="9" spans="2:9" ht="15" customHeight="1">
       <c r="B9" s="2"/>
-      <c r="C9" s="58"/>
-      <c r="D9" s="59"/>
-      <c r="E9" s="59"/>
-      <c r="F9" s="59"/>
-      <c r="G9" s="59"/>
+      <c r="C9" s="47"/>
+      <c r="D9" s="48"/>
+      <c r="E9" s="48"/>
+      <c r="F9" s="48"/>
+      <c r="G9" s="48"/>
     </row>
     <row r="10" spans="2:9" ht="7.5" customHeight="1">
       <c r="B10" s="2"/>
-      <c r="C10" s="58"/>
-      <c r="D10" s="59"/>
-      <c r="E10" s="59"/>
-      <c r="F10" s="59"/>
-      <c r="G10" s="59"/>
+      <c r="C10" s="47"/>
+      <c r="D10" s="48"/>
+      <c r="E10" s="48"/>
+      <c r="F10" s="48"/>
+      <c r="G10" s="48"/>
     </row>
     <row r="11" spans="2:9" hidden="1">
       <c r="B11" s="2"/>
-      <c r="C11" s="58"/>
-      <c r="D11" s="59"/>
-      <c r="E11" s="59"/>
-      <c r="F11" s="59"/>
-      <c r="G11" s="59"/>
+      <c r="C11" s="47"/>
+      <c r="D11" s="48"/>
+      <c r="E11" s="48"/>
+      <c r="F11" s="48"/>
+      <c r="G11" s="48"/>
     </row>
     <row r="12" spans="2:9" hidden="1">
       <c r="B12" s="4"/>
-      <c r="C12" s="58"/>
-      <c r="D12" s="59"/>
-      <c r="E12" s="59"/>
-      <c r="F12" s="59"/>
-      <c r="G12" s="59"/>
+      <c r="C12" s="47"/>
+      <c r="D12" s="48"/>
+      <c r="E12" s="48"/>
+      <c r="F12" s="48"/>
+      <c r="G12" s="48"/>
     </row>
     <row r="13" spans="2:9">
       <c r="B13" s="5"/>
-      <c r="C13" s="42" t="s">
+      <c r="C13" s="54" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="42"/>
-      <c r="E13" s="42"/>
-      <c r="F13" s="42"/>
-      <c r="G13" s="42"/>
+      <c r="D13" s="54"/>
+      <c r="E13" s="54"/>
+      <c r="F13" s="54"/>
+      <c r="G13" s="54"/>
     </row>
     <row r="14" spans="2:9">
       <c r="B14" s="5"/>
-      <c r="C14" s="43" t="s">
+      <c r="C14" s="55" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="44"/>
-      <c r="E14" s="45" t="s">
+      <c r="D14" s="56"/>
+      <c r="E14" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="F14" s="45"/>
-      <c r="G14" s="45"/>
+      <c r="F14" s="57"/>
+      <c r="G14" s="57"/>
     </row>
     <row r="15" spans="2:9">
       <c r="B15" s="4"/>
-      <c r="C15" s="40" t="s">
+      <c r="C15" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="D15" s="40"/>
-      <c r="E15" s="41"/>
-      <c r="F15" s="41"/>
-      <c r="G15" s="41"/>
+      <c r="D15" s="52"/>
+      <c r="E15" s="53"/>
+      <c r="F15" s="53"/>
+      <c r="G15" s="53"/>
     </row>
     <row r="16" spans="2:9" ht="24.95" customHeight="1">
       <c r="B16" s="6"/>
-      <c r="C16" s="38" t="s">
+      <c r="C16" s="58" t="s">
         <v>18</v>
       </c>
-      <c r="D16" s="39"/>
-      <c r="E16" s="37" t="s">
-        <v>75</v>
-      </c>
-      <c r="F16" s="37" t="s">
+      <c r="D16" s="59"/>
+      <c r="E16" s="60" t="s">
+        <v>73</v>
+      </c>
+      <c r="F16" s="60" t="s">
         <v>19</v>
       </c>
-      <c r="G16" s="37"/>
+      <c r="G16" s="60"/>
     </row>
     <row r="17" spans="2:7" ht="24.95" customHeight="1">
       <c r="B17" s="6"/>
-      <c r="C17" s="38" t="s">
+      <c r="C17" s="58" t="s">
         <v>20</v>
       </c>
-      <c r="D17" s="39"/>
-      <c r="E17" s="37" t="s">
+      <c r="D17" s="59"/>
+      <c r="E17" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="F17" s="37" t="s">
+      <c r="F17" s="60" t="s">
         <v>20</v>
       </c>
-      <c r="G17" s="37"/>
+      <c r="G17" s="60"/>
     </row>
     <row r="18" spans="2:7" ht="24.95" customHeight="1">
       <c r="B18" s="6"/>
-      <c r="C18" s="38" t="s">
+      <c r="C18" s="58" t="s">
         <v>22</v>
       </c>
-      <c r="D18" s="39"/>
-      <c r="E18" s="37" t="s">
-        <v>83</v>
-      </c>
-      <c r="F18" s="37" t="s">
+      <c r="D18" s="59"/>
+      <c r="E18" s="60" t="s">
+        <v>81</v>
+      </c>
+      <c r="F18" s="60" t="s">
         <v>23</v>
       </c>
-      <c r="G18" s="37"/>
+      <c r="G18" s="60"/>
     </row>
     <row r="19" spans="2:7" ht="24.95" customHeight="1">
       <c r="B19" s="6"/>
-      <c r="C19" s="38" t="s">
+      <c r="C19" s="58" t="s">
         <v>24</v>
       </c>
-      <c r="D19" s="39"/>
-      <c r="E19" s="37" t="s">
+      <c r="D19" s="59"/>
+      <c r="E19" s="60" t="s">
         <v>25</v>
       </c>
-      <c r="F19" s="37" t="s">
+      <c r="F19" s="60" t="s">
         <v>26</v>
       </c>
-      <c r="G19" s="37"/>
+      <c r="G19" s="60"/>
     </row>
     <row r="20" spans="2:7" ht="24.95" customHeight="1">
       <c r="B20" s="6"/>
-      <c r="C20" s="38" t="s">
+      <c r="C20" s="58" t="s">
         <v>27</v>
       </c>
-      <c r="D20" s="39"/>
-      <c r="E20" s="37" t="s">
+      <c r="D20" s="59"/>
+      <c r="E20" s="60" t="s">
         <v>28</v>
       </c>
-      <c r="F20" s="37" t="s">
+      <c r="F20" s="60" t="s">
         <v>28</v>
       </c>
-      <c r="G20" s="37"/>
+      <c r="G20" s="60"/>
     </row>
     <row r="21" spans="2:7" ht="24.95" customHeight="1">
       <c r="B21" s="6"/>
-      <c r="C21" s="38" t="s">
+      <c r="C21" s="58" t="s">
         <v>29</v>
       </c>
-      <c r="D21" s="39"/>
-      <c r="E21" s="37" t="s">
+      <c r="D21" s="59"/>
+      <c r="E21" s="60" t="s">
         <v>30</v>
       </c>
-      <c r="F21" s="37" t="s">
+      <c r="F21" s="60" t="s">
         <v>31</v>
       </c>
-      <c r="G21" s="37"/>
+      <c r="G21" s="60"/>
     </row>
     <row r="22" spans="2:7" ht="24.95" customHeight="1">
       <c r="B22" s="6"/>
-      <c r="C22" s="38" t="s">
+      <c r="C22" s="58" t="s">
         <v>32</v>
       </c>
-      <c r="D22" s="39"/>
-      <c r="E22" s="37" t="s">
+      <c r="D22" s="59"/>
+      <c r="E22" s="60" t="s">
         <v>33</v>
       </c>
-      <c r="F22" s="37"/>
-      <c r="G22" s="37"/>
+      <c r="F22" s="60"/>
+      <c r="G22" s="60"/>
     </row>
     <row r="23" spans="2:7" ht="24.95" customHeight="1">
       <c r="B23" s="6"/>
-      <c r="C23" s="38" t="s">
+      <c r="C23" s="58" t="s">
         <v>34</v>
       </c>
-      <c r="D23" s="39"/>
-      <c r="E23" s="37" t="s">
+      <c r="D23" s="59"/>
+      <c r="E23" s="60" t="s">
         <v>35</v>
       </c>
-      <c r="F23" s="37"/>
-      <c r="G23" s="37"/>
+      <c r="F23" s="60"/>
+      <c r="G23" s="60"/>
     </row>
     <row r="24" spans="2:7" ht="24.95" customHeight="1">
       <c r="B24" s="7"/>
-      <c r="C24" s="38" t="s">
+      <c r="C24" s="58" t="s">
         <v>36</v>
       </c>
-      <c r="D24" s="39"/>
-      <c r="E24" s="37" t="s">
+      <c r="D24" s="59"/>
+      <c r="E24" s="60" t="s">
         <v>37</v>
       </c>
-      <c r="F24" s="37" t="s">
+      <c r="F24" s="60" t="s">
         <v>38</v>
       </c>
-      <c r="G24" s="37"/>
+      <c r="G24" s="60"/>
     </row>
     <row r="25" spans="2:7" ht="24.95" customHeight="1">
       <c r="B25" s="7"/>
-      <c r="C25" s="38" t="s">
+      <c r="C25" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="D25" s="39"/>
-      <c r="E25" s="37" t="s">
+      <c r="D25" s="59"/>
+      <c r="E25" s="60" t="s">
         <v>39</v>
       </c>
-      <c r="F25" s="37" t="s">
+      <c r="F25" s="60" t="s">
         <v>40</v>
       </c>
-      <c r="G25" s="37"/>
+      <c r="G25" s="60"/>
     </row>
     <row r="26" spans="2:7" ht="24.95" customHeight="1">
       <c r="B26" s="6"/>
-      <c r="C26" s="38" t="s">
+      <c r="C26" s="58" t="s">
         <v>41</v>
       </c>
-      <c r="D26" s="39"/>
-      <c r="E26" s="37" t="s">
+      <c r="D26" s="59"/>
+      <c r="E26" s="60" t="s">
         <v>42</v>
       </c>
-      <c r="F26" s="37" t="s">
+      <c r="F26" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="G26" s="37"/>
+      <c r="G26" s="60"/>
     </row>
     <row r="27" spans="2:7" ht="24.95" customHeight="1">
       <c r="B27" s="7"/>
-      <c r="C27" s="38" t="s">
+      <c r="C27" s="58" t="s">
         <v>44</v>
       </c>
-      <c r="D27" s="39"/>
-      <c r="E27" s="37" t="s">
+      <c r="D27" s="59"/>
+      <c r="E27" s="60" t="s">
         <v>45</v>
       </c>
-      <c r="F27" s="37" t="s">
+      <c r="F27" s="60" t="s">
         <v>46</v>
       </c>
-      <c r="G27" s="37"/>
+      <c r="G27" s="60"/>
     </row>
     <row r="28" spans="2:7" ht="24.95" customHeight="1">
       <c r="B28" s="6"/>
-      <c r="C28" s="38" t="s">
+      <c r="C28" s="58" t="s">
         <v>47</v>
       </c>
-      <c r="D28" s="39"/>
-      <c r="E28" s="37" t="s">
+      <c r="D28" s="59"/>
+      <c r="E28" s="60" t="s">
         <v>48</v>
       </c>
-      <c r="F28" s="37" t="s">
+      <c r="F28" s="60" t="s">
         <v>49</v>
       </c>
-      <c r="G28" s="37"/>
+      <c r="G28" s="60"/>
     </row>
     <row r="29" spans="2:7" ht="24.95" customHeight="1">
       <c r="B29" s="8"/>
-      <c r="C29" s="35" t="s">
+      <c r="C29" s="61" t="s">
         <v>50</v>
       </c>
-      <c r="D29" s="36"/>
-      <c r="E29" s="37" t="s">
+      <c r="D29" s="62"/>
+      <c r="E29" s="60" t="s">
         <v>51</v>
       </c>
-      <c r="F29" s="37" t="s">
+      <c r="F29" s="60" t="s">
         <v>52</v>
       </c>
-      <c r="G29" s="37"/>
+      <c r="G29" s="60"/>
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="C3:G5"/>
-    <mergeCell ref="C6:G6"/>
-    <mergeCell ref="C8:C12"/>
-    <mergeCell ref="D8:G12"/>
-    <mergeCell ref="D7:G7"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="C13:G13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="E17:G17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="E18:G18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="E19:G19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="E20:G20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="E21:G21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="E22:G22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="E24:G24"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="E28:G28"/>
     <mergeCell ref="C29:D29"/>
     <mergeCell ref="E29:G29"/>
     <mergeCell ref="C25:D25"/>
@@ -2287,6 +2360,35 @@
     <mergeCell ref="E26:G26"/>
     <mergeCell ref="C27:D27"/>
     <mergeCell ref="E27:G27"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="E20:G20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="E21:G21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="E22:G22"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="E17:G17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="E18:G18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="E19:G19"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="C3:G5"/>
+    <mergeCell ref="C6:G6"/>
+    <mergeCell ref="C8:C12"/>
+    <mergeCell ref="D8:G12"/>
+    <mergeCell ref="D7:G7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -2296,10 +2398,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24:D24"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2319,217 +2421,274 @@
     </row>
     <row r="2" spans="1:7" ht="15" customHeight="1">
       <c r="A2" s="9"/>
-      <c r="B2" s="63" t="s">
+      <c r="B2" s="75" t="s">
         <v>53</v>
       </c>
-      <c r="C2" s="64"/>
-      <c r="D2" s="65"/>
+      <c r="C2" s="76"/>
+      <c r="D2" s="77"/>
       <c r="E2" s="14"/>
       <c r="F2" s="14"/>
       <c r="G2" s="10"/>
     </row>
     <row r="3" spans="1:7" ht="15" customHeight="1">
       <c r="A3" s="9"/>
-      <c r="B3" s="66"/>
-      <c r="C3" s="67"/>
-      <c r="D3" s="68"/>
+      <c r="B3" s="78"/>
+      <c r="C3" s="79"/>
+      <c r="D3" s="80"/>
       <c r="E3" s="14"/>
       <c r="F3" s="14"/>
       <c r="G3" s="10"/>
     </row>
     <row r="4" spans="1:7" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B4" s="69"/>
-      <c r="C4" s="70"/>
-      <c r="D4" s="71"/>
+      <c r="B4" s="81"/>
+      <c r="C4" s="82"/>
+      <c r="D4" s="83"/>
       <c r="E4" s="14"/>
       <c r="F4" s="14"/>
     </row>
     <row r="5" spans="1:7" ht="18">
-      <c r="B5" s="89" t="s">
+      <c r="B5" s="65" t="s">
         <v>54</v>
       </c>
-      <c r="C5" s="90"/>
-      <c r="D5" s="91"/>
+      <c r="C5" s="66"/>
+      <c r="D5" s="67"/>
     </row>
     <row r="6" spans="1:7" ht="15.75">
-      <c r="B6" s="94" t="s">
+      <c r="B6" s="72" t="s">
         <v>55</v>
       </c>
-      <c r="C6" s="95"/>
-      <c r="D6" s="96"/>
+      <c r="C6" s="73"/>
+      <c r="D6" s="74"/>
     </row>
     <row r="7" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="B7" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="C7" s="74" t="s">
+      <c r="C7" s="68" t="s">
         <v>57</v>
       </c>
-      <c r="D7" s="75"/>
+      <c r="D7" s="69"/>
     </row>
     <row r="8" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="B8" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="C8" s="74" t="s">
+      <c r="C8" s="68" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="75"/>
+      <c r="D8" s="69"/>
     </row>
     <row r="9" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="B9" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="C9" s="92" t="s">
+      <c r="C9" s="70" t="s">
         <v>60</v>
       </c>
-      <c r="D9" s="93"/>
+      <c r="D9" s="71"/>
     </row>
     <row r="10" spans="1:7" ht="32.25" customHeight="1">
       <c r="B10" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="C10" s="72">
+      <c r="C10" s="84">
         <v>42290</v>
       </c>
-      <c r="D10" s="73"/>
+      <c r="D10" s="85"/>
     </row>
     <row r="11" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="B11" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="C11" s="74" t="s">
+      <c r="C11" s="68" t="s">
         <v>63</v>
       </c>
-      <c r="D11" s="75"/>
+      <c r="D11" s="69"/>
     </row>
     <row r="12" spans="1:7" ht="33" customHeight="1">
       <c r="B12" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="C12" s="74" t="s">
-        <v>65</v>
-      </c>
-      <c r="D12" s="75"/>
+      <c r="C12" s="68" t="s">
+        <v>85</v>
+      </c>
+      <c r="D12" s="69"/>
     </row>
     <row r="13" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="B13" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="C13" s="70" t="s">
         <v>66</v>
       </c>
-      <c r="C13" s="92" t="s">
-        <v>67</v>
-      </c>
-      <c r="D13" s="93"/>
+      <c r="D13" s="71"/>
     </row>
     <row r="14" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="B14" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="C14" s="87" t="s">
-        <v>84</v>
-      </c>
-      <c r="D14" s="88"/>
+      <c r="C14" s="63" t="s">
+        <v>82</v>
+      </c>
+      <c r="D14" s="64"/>
     </row>
     <row r="15" spans="1:7">
-      <c r="B15" s="78" t="s">
+      <c r="B15" s="88" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="79"/>
-      <c r="D15" s="80"/>
+      <c r="C15" s="89"/>
+      <c r="D15" s="90"/>
     </row>
     <row r="16" spans="1:7" ht="50.1" customHeight="1">
-      <c r="B16" s="81" t="s">
+      <c r="B16" s="91" t="s">
+        <v>67</v>
+      </c>
+      <c r="C16" s="92"/>
+      <c r="D16" s="93"/>
+    </row>
+    <row r="17" spans="2:4">
+      <c r="B17" s="88" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" s="89"/>
+      <c r="D17" s="90"/>
+    </row>
+    <row r="18" spans="2:4" ht="50.1" customHeight="1">
+      <c r="B18" s="91" t="s">
         <v>68</v>
       </c>
-      <c r="C16" s="82"/>
-      <c r="D16" s="83"/>
-    </row>
-    <row r="17" spans="2:4">
-      <c r="B17" s="78" t="s">
-        <v>13</v>
-      </c>
-      <c r="C17" s="79"/>
-      <c r="D17" s="80"/>
-    </row>
-    <row r="18" spans="2:4" ht="50.1" customHeight="1">
-      <c r="B18" s="81" t="s">
+      <c r="C18" s="92"/>
+      <c r="D18" s="93"/>
+    </row>
+    <row r="19" spans="2:4">
+      <c r="B19" s="88" t="s">
         <v>69</v>
       </c>
-      <c r="C18" s="82"/>
-      <c r="D18" s="83"/>
-    </row>
-    <row r="19" spans="2:4">
-      <c r="B19" s="78" t="s">
+      <c r="C19" s="89"/>
+      <c r="D19" s="90"/>
+    </row>
+    <row r="20" spans="2:4" ht="50.1" customHeight="1">
+      <c r="B20" s="91" t="s">
+        <v>83</v>
+      </c>
+      <c r="C20" s="92"/>
+      <c r="D20" s="93"/>
+    </row>
+    <row r="21" spans="2:4">
+      <c r="B21" s="88" t="s">
         <v>70</v>
       </c>
-      <c r="C19" s="79"/>
-      <c r="D19" s="80"/>
-    </row>
-    <row r="20" spans="2:4" ht="50.1" customHeight="1">
-      <c r="B20" s="81" t="s">
-        <v>85</v>
-      </c>
-      <c r="C20" s="82"/>
-      <c r="D20" s="83"/>
-    </row>
-    <row r="21" spans="2:4">
-      <c r="B21" s="78" t="s">
+      <c r="C21" s="89"/>
+      <c r="D21" s="90"/>
+    </row>
+    <row r="22" spans="2:4" ht="50.1" customHeight="1">
+      <c r="B22" s="91" t="s">
+        <v>74</v>
+      </c>
+      <c r="C22" s="92"/>
+      <c r="D22" s="93"/>
+    </row>
+    <row r="23" spans="2:4" ht="15.75" thickBot="1">
+      <c r="B23" s="94" t="s">
+        <v>47</v>
+      </c>
+      <c r="C23" s="95"/>
+      <c r="D23" s="96"/>
+    </row>
+    <row r="24" spans="2:4" ht="36" customHeight="1">
+      <c r="B24" s="101" t="s">
+        <v>86</v>
+      </c>
+      <c r="C24" s="102"/>
+      <c r="D24" s="103"/>
+    </row>
+    <row r="25" spans="2:4" ht="15" customHeight="1">
+      <c r="B25" s="104" t="s">
+        <v>87</v>
+      </c>
+      <c r="C25" s="97"/>
+      <c r="D25" s="105"/>
+    </row>
+    <row r="26" spans="2:4" ht="15" customHeight="1">
+      <c r="B26" s="104" t="s">
+        <v>88</v>
+      </c>
+      <c r="C26" s="97"/>
+      <c r="D26" s="105"/>
+    </row>
+    <row r="27" spans="2:4" ht="15" customHeight="1">
+      <c r="B27" s="104" t="s">
+        <v>89</v>
+      </c>
+      <c r="C27" s="97"/>
+      <c r="D27" s="105"/>
+    </row>
+    <row r="28" spans="2:4" ht="15" customHeight="1">
+      <c r="B28" s="104" t="s">
+        <v>90</v>
+      </c>
+      <c r="C28" s="97"/>
+      <c r="D28" s="105"/>
+    </row>
+    <row r="29" spans="2:4" ht="15" customHeight="1">
+      <c r="B29" s="104" t="s">
+        <v>91</v>
+      </c>
+      <c r="C29" s="97"/>
+      <c r="D29" s="105"/>
+    </row>
+    <row r="30" spans="2:4" ht="15" customHeight="1">
+      <c r="B30" s="104" t="s">
+        <v>92</v>
+      </c>
+      <c r="C30" s="97"/>
+      <c r="D30" s="105"/>
+    </row>
+    <row r="31" spans="2:4" ht="15" customHeight="1">
+      <c r="B31" s="104" t="s">
+        <v>93</v>
+      </c>
+      <c r="C31" s="97"/>
+      <c r="D31" s="105"/>
+    </row>
+    <row r="32" spans="2:4" ht="15" customHeight="1" thickBot="1">
+      <c r="B32" s="106" t="s">
+        <v>94</v>
+      </c>
+      <c r="C32" s="107"/>
+      <c r="D32" s="108"/>
+    </row>
+    <row r="33" spans="2:4" ht="15.75" thickBot="1">
+      <c r="B33" s="98" t="s">
         <v>71</v>
       </c>
-      <c r="C21" s="79"/>
-      <c r="D21" s="80"/>
-    </row>
-    <row r="22" spans="2:4" ht="50.1" customHeight="1">
-      <c r="B22" s="81" t="s">
-        <v>76</v>
-      </c>
-      <c r="C22" s="82"/>
-      <c r="D22" s="83"/>
-    </row>
-    <row r="23" spans="2:4">
-      <c r="B23" s="78" t="s">
-        <v>47</v>
-      </c>
-      <c r="C23" s="79"/>
-      <c r="D23" s="80"/>
-    </row>
-    <row r="24" spans="2:4" ht="50.1" customHeight="1">
-      <c r="B24" s="81" t="s">
+      <c r="C33" s="99"/>
+      <c r="D33" s="100"/>
+    </row>
+    <row r="34" spans="2:4" ht="26.25" thickBot="1">
+      <c r="B34" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="C24" s="82"/>
-      <c r="D24" s="83"/>
-    </row>
-    <row r="25" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B25" s="84" t="s">
-        <v>73</v>
-      </c>
-      <c r="C25" s="85"/>
-      <c r="D25" s="86"/>
-    </row>
-    <row r="26" spans="2:4" ht="26.25" thickBot="1">
-      <c r="B26" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="C26" s="76" t="s">
-        <v>77</v>
-      </c>
-      <c r="D26" s="77"/>
+      <c r="C34" s="86" t="s">
+        <v>75</v>
+      </c>
+      <c r="D34" s="87"/>
     </row>
   </sheetData>
-  <mergeCells count="23">
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="C13:D13"/>
+  <mergeCells count="31">
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="B31:D31"/>
     <mergeCell ref="B2:D4"/>
     <mergeCell ref="C10:D10"/>
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C34:D34"/>
     <mergeCell ref="B15:D15"/>
     <mergeCell ref="B16:D16"/>
     <mergeCell ref="B17:D17"/>
@@ -2540,7 +2699,14 @@
     <mergeCell ref="B22:D22"/>
     <mergeCell ref="B23:D23"/>
     <mergeCell ref="B24:D24"/>
-    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="C13:D13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>